<commit_message>
Updated ePU and eBF
</commit_message>
<xml_diff>
--- a/eBF Compiler and Parser.xlsx
+++ b/eBF Compiler and Parser.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SENGa\ePU\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55C0EBAD-3077-4ED8-B995-2EF7AFD24DB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0BF592D-B3ED-4ACD-AD17-2C222F818013}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{B06A63A8-6D73-4E43-885F-3569BFC944DC}"/>
   </bookViews>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
   <si>
     <t>PROGRAM START</t>
   </si>
@@ -109,9 +109,6 @@
   </si>
   <si>
     <t>0001</t>
-  </si>
-  <si>
-    <t>0000</t>
   </si>
   <si>
     <t>0010</t>
@@ -229,7 +226,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -347,12 +344,23 @@
     </border>
     <border>
       <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -362,24 +370,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -395,6 +398,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -732,7 +741,7 @@
   <dimension ref="B1:Y26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -744,140 +753,98 @@
       <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="13"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+    </row>
+    <row r="2" spans="2:25" x14ac:dyDescent="0.3">
+      <c r="E2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="2:25" x14ac:dyDescent="0.3">
-      <c r="E2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" s="18" t="s">
+      <c r="G2" s="13"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+    </row>
+    <row r="3" spans="2:25" x14ac:dyDescent="0.3">
+      <c r="E3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="2:25" x14ac:dyDescent="0.3">
-      <c r="E3" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" s="18" t="s">
+      <c r="G3" s="13"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+    </row>
+    <row r="4" spans="2:25" x14ac:dyDescent="0.3">
+      <c r="E4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="2:25" x14ac:dyDescent="0.3">
-      <c r="E4" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F4" s="18" t="s">
+      <c r="G4" s="13"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="K4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="2:25" x14ac:dyDescent="0.3">
+      <c r="E5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K4" s="11" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="2:25" x14ac:dyDescent="0.3">
-      <c r="E5" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F5" s="18" t="s">
+      <c r="G5" s="13"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="O5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="2:25" x14ac:dyDescent="0.3">
+      <c r="E6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="G5" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I5" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="O5" t="s">
+      <c r="G6" s="13"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="9"/>
+      <c r="Q6" s="9" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="6" spans="2:25" x14ac:dyDescent="0.3">
-      <c r="E6" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F6" s="18" t="s">
+      <c r="R6" s="9"/>
+      <c r="S6" s="9"/>
+      <c r="T6" s="9"/>
+      <c r="U6" s="9"/>
+      <c r="V6" s="9"/>
+      <c r="W6" s="9"/>
+      <c r="X6" s="9"/>
+      <c r="Y6" s="17"/>
+    </row>
+    <row r="7" spans="2:25" x14ac:dyDescent="0.3">
+      <c r="E7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="G6" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I6" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="O6" s="1"/>
-      <c r="P6" s="12"/>
-      <c r="Q6" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="R6" s="12"/>
-      <c r="S6" s="12"/>
-      <c r="T6" s="12"/>
-      <c r="U6" s="12"/>
-      <c r="V6" s="12"/>
-      <c r="W6" s="12"/>
-      <c r="X6" s="12"/>
-      <c r="Y6" s="22"/>
-    </row>
-    <row r="7" spans="2:25" x14ac:dyDescent="0.3">
-      <c r="E7" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F7" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I7" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="O7" s="4"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="O7" s="3"/>
       <c r="Q7">
         <v>1</v>
       </c>
@@ -892,264 +859,258 @@
       </c>
       <c r="W7" cm="1">
         <f t="array" aca="1" ref="W7" ca="1">INDIRECT(ADDRESS(V10, V9 + S11))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X7" t="s">
-        <v>35</v>
-      </c>
-      <c r="Y7" s="23"/>
+        <v>34</v>
+      </c>
+      <c r="Y7" s="18"/>
     </row>
     <row r="8" spans="2:25" x14ac:dyDescent="0.3">
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="21">
+      <c r="F8" s="16">
         <v>1000</v>
       </c>
-      <c r="G8" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H8" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="I8" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="O8" s="4"/>
-      <c r="Y8" s="23"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="O8" s="3"/>
+      <c r="Y8" s="18"/>
     </row>
     <row r="9" spans="2:25" x14ac:dyDescent="0.3">
-      <c r="F9" s="13"/>
-      <c r="O9" s="4"/>
+      <c r="O9" s="3"/>
       <c r="Q9">
         <v>1010</v>
       </c>
       <c r="R9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="V9">
         <v>16</v>
       </c>
       <c r="W9" t="s">
-        <v>37</v>
-      </c>
-      <c r="Y9" s="23"/>
+        <v>36</v>
+      </c>
+      <c r="Y9" s="18"/>
     </row>
     <row r="10" spans="2:25" x14ac:dyDescent="0.3">
       <c r="E10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F10" s="19">
+      <c r="F10" s="14">
         <v>1001</v>
       </c>
-      <c r="G10" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="O10" s="4"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="O10" s="3"/>
       <c r="V10">
         <v>7</v>
       </c>
       <c r="W10" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y10" s="18"/>
+    </row>
+    <row r="11" spans="2:25" x14ac:dyDescent="0.3">
+      <c r="E11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="15">
+        <v>1010</v>
+      </c>
+      <c r="G11" s="21"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="O11" s="3" t="s">
         <v>38</v>
-      </c>
-      <c r="Y10" s="23"/>
-    </row>
-    <row r="11" spans="2:25" x14ac:dyDescent="0.3">
-      <c r="E11" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F11" s="20">
-        <v>1010</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I11" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="O11" s="4" t="s">
-        <v>39</v>
       </c>
       <c r="Q11" t="str">
         <f ca="1">MID(Q9, S11, 1)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S11">
         <f ca="1">IF(J20 = 1, IF(S11 = (LEN(Q9) + 1), 1, S11 + 1),  S11)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T11" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y11" s="23"/>
+        <v>39</v>
+      </c>
+      <c r="Y11" s="18"/>
     </row>
     <row r="12" spans="2:25" x14ac:dyDescent="0.3">
-      <c r="E12" s="4" t="s">
+      <c r="E12" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F12" s="20">
+      <c r="F12" s="15">
         <v>1011</v>
       </c>
-      <c r="G12" s="13" t="s">
+      <c r="G12" t="s">
+        <v>22</v>
+      </c>
+      <c r="H12" t="s">
         <v>23</v>
       </c>
-      <c r="H12" s="13" t="s">
+      <c r="I12" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="I12" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="O12" s="4"/>
-      <c r="Y12" s="23"/>
+      <c r="L12" s="4"/>
+      <c r="O12" s="3"/>
+      <c r="Y12" s="18"/>
     </row>
     <row r="13" spans="2:25" x14ac:dyDescent="0.3">
-      <c r="E13" s="4" t="s">
+      <c r="E13" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F13" s="20">
+      <c r="F13" s="15">
         <v>1100</v>
       </c>
-      <c r="G13" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I13" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K13" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="O13" s="4"/>
+      <c r="G13" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H13" s="22"/>
+      <c r="I13" s="23"/>
+      <c r="K13" t="s">
+        <v>28</v>
+      </c>
+      <c r="O13" s="3"/>
       <c r="Q13">
         <v>1</v>
       </c>
       <c r="R13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="V13" t="str">
         <f>_xlfn.CONCAT(Q7,R7,S7,T7)</f>
         <v>1010</v>
       </c>
-      <c r="W13" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="Y13" s="23"/>
+      <c r="W13" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y13" s="18"/>
     </row>
     <row r="14" spans="2:25" x14ac:dyDescent="0.3">
-      <c r="E14" s="4" t="s">
+      <c r="E14" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F14" s="20">
+      <c r="F14" s="15">
         <v>1101</v>
       </c>
-      <c r="G14" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="H14" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="I14" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="O14" s="4"/>
+      <c r="G14" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="O14" s="3"/>
       <c r="V14">
         <f>BIN2DEC(V13)</f>
         <v>10</v>
       </c>
-      <c r="W14" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="Y14" s="23"/>
+      <c r="W14" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y14" s="18"/>
     </row>
     <row r="15" spans="2:25" x14ac:dyDescent="0.3">
-      <c r="E15" s="4" t="s">
+      <c r="E15" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F15" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="H15" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="I15" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="O15" s="4"/>
+      <c r="F15" s="24">
+        <v>1110</v>
+      </c>
+      <c r="G15" s="23"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="O15" s="3"/>
       <c r="Q15">
         <f ca="1">IF(J20 = 1, IF(Q15 &gt;= Q13, 0, Q15 + 1), Q15)</f>
         <v>0</v>
       </c>
       <c r="S15" t="str">
         <f ca="1">IF(Q15 = Q13, IF(LEN(S15) = LEN(Q9), "", S15 &amp; Q11), S15)</f>
-        <v>101</v>
-      </c>
-      <c r="Y15" s="23"/>
+        <v>10</v>
+      </c>
+      <c r="Y15" s="18"/>
     </row>
     <row r="16" spans="2:25" x14ac:dyDescent="0.3">
-      <c r="E16" s="14" t="s">
+      <c r="E16" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F16" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="F16" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="G16" s="16"/>
-      <c r="O16" s="7"/>
-      <c r="P16" s="8"/>
-      <c r="Q16" s="8" t="s">
+      <c r="G16" s="20"/>
+      <c r="O16" s="6"/>
+      <c r="P16" s="7"/>
+      <c r="Q16" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="R16" s="7"/>
+      <c r="S16" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="R16" s="8"/>
-      <c r="S16" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="T16" s="8"/>
-      <c r="U16" s="8"/>
-      <c r="V16" s="8"/>
-      <c r="W16" s="8"/>
-      <c r="X16" s="8"/>
-      <c r="Y16" s="25"/>
-    </row>
-    <row r="20" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="T16" s="7"/>
+      <c r="U16" s="7"/>
+      <c r="V16" s="7"/>
+      <c r="W16" s="7"/>
+      <c r="X16" s="7"/>
+      <c r="Y16" s="20"/>
+    </row>
+    <row r="18" spans="4:20" x14ac:dyDescent="0.3">
+      <c r="K18" s="4"/>
+      <c r="N18" s="4"/>
+      <c r="O18" s="4"/>
+      <c r="Q18" s="4"/>
+      <c r="R18" s="4"/>
+      <c r="S18" s="4"/>
+      <c r="T18" s="4"/>
+    </row>
+    <row r="20" spans="4:20" x14ac:dyDescent="0.3">
       <c r="J20">
         <f ca="1">IF(J20=0, 1, 0)</f>
         <v>0</v>
       </c>
       <c r="K20" t="s">
+        <v>29</v>
+      </c>
+      <c r="O20" s="4"/>
+      <c r="P20" s="4"/>
+      <c r="R20" s="4"/>
+    </row>
+    <row r="21" spans="4:20" x14ac:dyDescent="0.3">
+      <c r="R21" s="4"/>
+    </row>
+    <row r="22" spans="4:20" x14ac:dyDescent="0.3">
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
+      <c r="N22" s="4"/>
+      <c r="Q22" s="4"/>
+    </row>
+    <row r="23" spans="4:20" x14ac:dyDescent="0.3">
+      <c r="F23" s="4"/>
+    </row>
+    <row r="26" spans="4:20" x14ac:dyDescent="0.3">
+      <c r="D26" t="s">
+        <v>31</v>
+      </c>
+      <c r="F26" s="4">
+        <v>1111</v>
+      </c>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4"/>
+      <c r="J26" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="26" spans="4:11" x14ac:dyDescent="0.3">
-      <c r="D26" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="F26" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G26" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="H26" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I26" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="J26" s="11" t="s">
-        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed RAM Unit from x4 to x16 Started work on eBF compiler Updated README.md and PDF Updated eBF2eBin.png
</commit_message>
<xml_diff>
--- a/eBF Compiler and Parser.xlsx
+++ b/eBF Compiler and Parser.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SENGa\ePU\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sebastian\ePU\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0BF592D-B3ED-4ACD-AD17-2C222F818013}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C327AFFC-25E1-4B6B-87E6-07861F317D22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{B06A63A8-6D73-4E43-885F-3569BFC944DC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{B06A63A8-6D73-4E43-885F-3569BFC944DC}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Working Sheet and Dev Notes" sheetId="1" r:id="rId1"/>
+    <sheet name="Final Build" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="CLOCK">Sheet1!$A$1</definedName>
+    <definedName name="CLOCK">'Working Sheet and Dev Notes'!$A$29</definedName>
   </definedNames>
   <calcPr calcId="191029" iterate="1" iterateCount="1"/>
   <extLst>
@@ -61,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="80">
   <si>
     <t>PROGRAM START</t>
   </si>
@@ -129,12 +130,6 @@
     <t>0111</t>
   </si>
   <si>
-    <t>XXXX</t>
-  </si>
-  <si>
-    <t>YYYY</t>
-  </si>
-  <si>
     <t>----</t>
   </si>
   <si>
@@ -196,6 +191,117 @@
   </si>
   <si>
     <t>OUTPUT</t>
+  </si>
+  <si>
+    <t>1011</t>
+  </si>
+  <si>
+    <t>1100</t>
+  </si>
+  <si>
+    <t>1110</t>
+  </si>
+  <si>
+    <t>exBin</t>
+  </si>
+  <si>
+    <t>Sphere</t>
+  </si>
+  <si>
+    <t>=</t>
+  </si>
+  <si>
+    <t>x86 ASM</t>
+  </si>
+  <si>
+    <t>Machine Code</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>NOTES:</t>
+  </si>
+  <si>
+    <t>Always write your DPND tokens first</t>
+  </si>
+  <si>
+    <t>It makes the PC faster</t>
+  </si>
+  <si>
+    <t>As it won't have to stop in the middle of processing to ask the Registers to load in more from the ROM</t>
+  </si>
+  <si>
+    <t>x86x64</t>
+  </si>
+  <si>
+    <t>ePUx4</t>
+  </si>
+  <si>
+    <t>Description of code</t>
+  </si>
+  <si>
+    <t>End Program</t>
+  </si>
+  <si>
+    <t>Load in Address 0011 0001 to Registers with Alias "0001"</t>
+  </si>
+  <si>
+    <t>Run program located at Alias "0001"</t>
+  </si>
+  <si>
+    <t>Write Pointer value to RAM at position of Pointer</t>
+  </si>
+  <si>
+    <t>Increment Pointer value</t>
+  </si>
+  <si>
+    <t>Increment Pointer position</t>
+  </si>
+  <si>
+    <t>Decrement Pointer position</t>
+  </si>
+  <si>
+    <t>Pointer.value++;</t>
+  </si>
+  <si>
+    <t>Pointer.position++;</t>
+  </si>
+  <si>
+    <t>Pointer.position--;</t>
+  </si>
+  <si>
+    <t>Run(0001);</t>
+  </si>
+  <si>
+    <t>Program 0001 = Address(0011, 0001);</t>
+  </si>
+  <si>
+    <t>Return 0;</t>
+  </si>
+  <si>
+    <t>Psuedo-code</t>
+  </si>
+  <si>
+    <t>RAM(Pointer.position, Pointer.value);</t>
+  </si>
+  <si>
+    <t>(I'm swapping the commands for output and input because I prefer these symbols swapped)</t>
+  </si>
+  <si>
+    <t>eBin</t>
+  </si>
+  <si>
+    <t>ALIAS</t>
+  </si>
+  <si>
+    <t>XXXXXXXX</t>
+  </si>
+  <si>
+    <t>YYYYYYYY</t>
+  </si>
+  <si>
+    <t>PROGRAM POINTER</t>
   </si>
 </sst>
 </file>
@@ -226,7 +332,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -366,17 +472,53 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyBorder="1"/>
@@ -404,6 +546,114 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -738,110 +988,119 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EE5DD05-ADC3-4927-894B-E00B418CFE20}">
-  <dimension ref="B1:Y26"/>
+  <dimension ref="A1:Y46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="2:25" x14ac:dyDescent="0.3">
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="1" t="s">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A1" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="E1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A2" s="61" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="13"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-    </row>
-    <row r="2" spans="2:25" x14ac:dyDescent="0.3">
-      <c r="E2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" s="13"/>
+      <c r="G2" s="12"/>
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
     </row>
-    <row r="3" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A3" s="61" t="s">
+        <v>1</v>
+      </c>
       <c r="E3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" s="13"/>
+        <v>2</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="12"/>
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
     </row>
-    <row r="4" spans="2:25" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A4" s="61" t="s">
+        <v>1</v>
+      </c>
       <c r="E4" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F4" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" s="13"/>
+        <v>3</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="12"/>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
-      <c r="K4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="2:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A5" s="61" t="s">
+        <v>1</v>
+      </c>
       <c r="E5" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F5" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" s="13"/>
+        <v>4</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="12"/>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
       <c r="O5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="2:25" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="61" t="s">
+        <v>3</v>
+      </c>
       <c r="E6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F6" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6" s="13"/>
+        <v>5</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" s="12"/>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
       <c r="O6" s="1"/>
-      <c r="P6" s="9"/>
-      <c r="Q6" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="R6" s="9"/>
-      <c r="S6" s="9"/>
-      <c r="T6" s="9"/>
-      <c r="U6" s="9"/>
-      <c r="V6" s="9"/>
-      <c r="W6" s="9"/>
-      <c r="X6" s="9"/>
-      <c r="Y6" s="17"/>
-    </row>
-    <row r="7" spans="2:25" x14ac:dyDescent="0.3">
+      <c r="P6" s="8"/>
+      <c r="Q6" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="R6" s="8"/>
+      <c r="S6" s="8"/>
+      <c r="T6" s="8"/>
+      <c r="U6" s="8"/>
+      <c r="V6" s="8"/>
+      <c r="W6" s="8"/>
+      <c r="X6" s="8"/>
+      <c r="Y6" s="16"/>
+    </row>
+    <row r="7" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="61" t="s">
+        <v>3</v>
+      </c>
       <c r="E7" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F7" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="G7" s="13"/>
+        <v>6</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="12"/>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
       <c r="O7" s="3"/>
@@ -862,70 +1121,91 @@
         <v>0</v>
       </c>
       <c r="X7" t="s">
-        <v>34</v>
-      </c>
-      <c r="Y7" s="18"/>
-    </row>
-    <row r="8" spans="2:25" x14ac:dyDescent="0.3">
-      <c r="E8" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y7" s="17"/>
+    </row>
+    <row r="8" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="61" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="H8" s="57"/>
+      <c r="I8" s="57"/>
+      <c r="J8" s="57"/>
+      <c r="K8" s="57"/>
+      <c r="O8" s="3"/>
+      <c r="Y8" s="17"/>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A9" s="61" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="16">
+      <c r="F9" s="15">
         <v>1000</v>
       </c>
-      <c r="G8" s="13"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="O8" s="3"/>
-      <c r="Y8" s="18"/>
-    </row>
-    <row r="9" spans="2:25" x14ac:dyDescent="0.3">
+      <c r="G9" s="29"/>
+      <c r="H9" s="57"/>
+      <c r="I9" s="57"/>
+      <c r="J9" s="57"/>
+      <c r="K9" s="57"/>
       <c r="O9" s="3"/>
       <c r="Q9">
         <v>1010</v>
       </c>
       <c r="R9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="V9">
         <v>16</v>
       </c>
       <c r="W9" t="s">
-        <v>36</v>
-      </c>
-      <c r="Y9" s="18"/>
-    </row>
-    <row r="10" spans="2:25" x14ac:dyDescent="0.3">
-      <c r="E10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" s="14">
-        <v>1001</v>
-      </c>
-      <c r="G10" s="13"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
+        <v>34</v>
+      </c>
+      <c r="Y9" s="17"/>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A10" s="61" t="s">
+        <v>4</v>
+      </c>
+      <c r="E10" t="s">
+        <v>26</v>
+      </c>
       <c r="O10" s="3"/>
       <c r="V10">
         <v>7</v>
       </c>
       <c r="W10" t="s">
-        <v>37</v>
-      </c>
-      <c r="Y10" s="18"/>
-    </row>
-    <row r="11" spans="2:25" x14ac:dyDescent="0.3">
-      <c r="E11" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F11" s="15">
-        <v>1010</v>
-      </c>
-      <c r="G11" s="21"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
+        <v>35</v>
+      </c>
+      <c r="Y10" s="17"/>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A11" s="61" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="13">
+        <v>1001</v>
+      </c>
+      <c r="G11" s="12"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
       <c r="O11" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="Q11" t="str">
         <f ca="1">MID(Q9, S11, 1)</f>
@@ -933,100 +1213,117 @@
       </c>
       <c r="S11">
         <f ca="1">IF(J20 = 1, IF(S11 = (LEN(Q9) + 1), 1, S11 + 1),  S11)</f>
+        <v>5</v>
+      </c>
+      <c r="T11" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y11" s="17"/>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A12" s="61" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" s="14">
+        <v>1010</v>
+      </c>
+      <c r="G12" s="20"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="55"/>
+      <c r="O12" s="3"/>
+      <c r="Y12" s="17"/>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A13" s="61" t="s">
         <v>3</v>
       </c>
-      <c r="T11" t="s">
-        <v>39</v>
-      </c>
-      <c r="Y11" s="18"/>
-    </row>
-    <row r="12" spans="2:25" x14ac:dyDescent="0.3">
-      <c r="E12" s="3" t="s">
+      <c r="E13" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F12" s="15">
+      <c r="F13" s="14">
         <v>1011</v>
       </c>
-      <c r="G12" t="s">
-        <v>22</v>
-      </c>
-      <c r="H12" t="s">
-        <v>23</v>
-      </c>
-      <c r="I12" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="L12" s="4"/>
-      <c r="O12" s="3"/>
-      <c r="Y12" s="18"/>
-    </row>
-    <row r="13" spans="2:25" x14ac:dyDescent="0.3">
-      <c r="E13" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F13" s="15">
-        <v>1100</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="H13" s="22"/>
-      <c r="I13" s="23"/>
-      <c r="K13" t="s">
-        <v>28</v>
-      </c>
+      <c r="G13" s="49" t="s">
+        <v>77</v>
+      </c>
+      <c r="H13" s="49"/>
+      <c r="I13" s="56" t="s">
+        <v>78</v>
+      </c>
+      <c r="J13" s="56"/>
+      <c r="K13" s="37" t="s">
+        <v>76</v>
+      </c>
+      <c r="L13" s="38"/>
       <c r="O13" s="3"/>
       <c r="Q13">
         <v>1</v>
       </c>
       <c r="R13" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="V13" t="str">
         <f>_xlfn.CONCAT(Q7,R7,S7,T7)</f>
         <v>1010</v>
       </c>
-      <c r="W13" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="Y13" s="18"/>
-    </row>
-    <row r="14" spans="2:25" x14ac:dyDescent="0.3">
+      <c r="W13" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y13" s="17"/>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A14" s="61" t="s">
+        <v>3</v>
+      </c>
       <c r="E14" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F14" s="15">
-        <v>1101</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="H14" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="I14" s="5" t="s">
-        <v>24</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="F14" s="14">
+        <v>1100</v>
+      </c>
+      <c r="G14" s="53" t="s">
+        <v>76</v>
+      </c>
+      <c r="H14" s="52"/>
+      <c r="I14" s="21"/>
       <c r="O14" s="3"/>
       <c r="V14">
         <f>BIN2DEC(V13)</f>
         <v>10</v>
       </c>
-      <c r="W14" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="Y14" s="18"/>
-    </row>
-    <row r="15" spans="2:25" x14ac:dyDescent="0.3">
+      <c r="W14" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y14" s="17"/>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A15" s="61" t="s">
+        <v>7</v>
+      </c>
       <c r="E15" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F15" s="24">
-        <v>1110</v>
-      </c>
-      <c r="G15" s="23"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
+        <v>13</v>
+      </c>
+      <c r="F15" s="14">
+        <v>1101</v>
+      </c>
+      <c r="G15" s="51" t="s">
+        <v>22</v>
+      </c>
+      <c r="H15" s="54" t="s">
+        <v>22</v>
+      </c>
+      <c r="I15" s="54"/>
+      <c r="J15" s="56" t="s">
+        <v>22</v>
+      </c>
+      <c r="K15" s="56"/>
+      <c r="L15" s="56" t="s">
+        <v>22</v>
+      </c>
+      <c r="M15" s="58"/>
       <c r="O15" s="3"/>
       <c r="Q15">
         <f ca="1">IF(J20 = 1, IF(Q15 &gt;= Q13, 0, Q15 + 1), Q15)</f>
@@ -1034,36 +1331,68 @@
       </c>
       <c r="S15" t="str">
         <f ca="1">IF(Q15 = Q13, IF(LEN(S15) = LEN(Q9), "", S15 &amp; Q11), S15)</f>
-        <v>10</v>
-      </c>
-      <c r="Y15" s="18"/>
-    </row>
-    <row r="16" spans="2:25" x14ac:dyDescent="0.3">
-      <c r="E16" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="F16" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="G16" s="20"/>
-      <c r="O16" s="6"/>
-      <c r="P16" s="7"/>
-      <c r="Q16" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="R16" s="7"/>
-      <c r="S16" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="T16" s="7"/>
-      <c r="U16" s="7"/>
-      <c r="V16" s="7"/>
-      <c r="W16" s="7"/>
-      <c r="X16" s="7"/>
-      <c r="Y16" s="20"/>
-    </row>
-    <row r="18" spans="4:20" x14ac:dyDescent="0.3">
-      <c r="K18" s="4"/>
+        <v>1010</v>
+      </c>
+      <c r="Y15" s="17"/>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A16" s="61" t="s">
+        <v>4</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16" s="23">
+        <v>1110</v>
+      </c>
+      <c r="G16" s="22"/>
+      <c r="O16" s="5"/>
+      <c r="P16" s="6"/>
+      <c r="Q16" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="R16" s="6"/>
+      <c r="S16" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="T16" s="6"/>
+      <c r="U16" s="6"/>
+      <c r="V16" s="6"/>
+      <c r="W16" s="6"/>
+      <c r="X16" s="6"/>
+      <c r="Y16" s="19"/>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A17" s="61" t="s">
+        <v>2</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G17" s="19"/>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A18" s="61" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="F18" s="37"/>
+      <c r="G18" s="59">
+        <v>1111</v>
+      </c>
+      <c r="H18" s="37" t="s">
+        <v>28</v>
+      </c>
+      <c r="I18" s="37"/>
+      <c r="J18" s="37"/>
+      <c r="K18" s="37"/>
+      <c r="L18" s="37"/>
+      <c r="M18" s="38"/>
       <c r="N18" s="4"/>
       <c r="O18" s="4"/>
       <c r="Q18" s="4"/>
@@ -1071,49 +1400,499 @@
       <c r="S18" s="4"/>
       <c r="T18" s="4"/>
     </row>
-    <row r="20" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A19" s="61" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A20" s="61" t="s">
+        <v>3</v>
+      </c>
       <c r="J20">
         <f ca="1">IF(J20=0, 1, 0)</f>
         <v>0</v>
       </c>
       <c r="K20" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="O20" s="4"/>
       <c r="P20" s="4"/>
       <c r="R20" s="4"/>
     </row>
-    <row r="21" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A21" s="61" t="s">
+        <v>1</v>
+      </c>
+      <c r="E21" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="F21" s="28"/>
+      <c r="G21" s="37" t="s">
+        <v>56</v>
+      </c>
+      <c r="H21" s="38"/>
       <c r="R21" s="4"/>
     </row>
-    <row r="22" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A22" s="61" t="s">
+        <v>1</v>
+      </c>
       <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
+      <c r="E22" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="F22" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="G22" s="48" t="s">
+        <v>50</v>
+      </c>
+      <c r="H22" s="50"/>
       <c r="I22" s="4"/>
       <c r="N22" s="4"/>
       <c r="Q22" s="4"/>
     </row>
-    <row r="23" spans="4:20" x14ac:dyDescent="0.3">
-      <c r="F23" s="4"/>
-    </row>
-    <row r="26" spans="4:20" x14ac:dyDescent="0.3">
-      <c r="D26" t="s">
-        <v>31</v>
-      </c>
-      <c r="F26" s="4">
-        <v>1111</v>
-      </c>
-      <c r="G26" s="4"/>
-      <c r="H26" s="4"/>
-      <c r="I26" s="4"/>
-      <c r="J26" t="s">
-        <v>30</v>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A23" s="61" t="s">
+        <v>1</v>
+      </c>
+      <c r="E23" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="F23" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="G23" s="42" t="s">
+        <v>49</v>
+      </c>
+      <c r="H23" s="44"/>
+      <c r="U23">
+        <f ca="1">IF(J20 = 1, IF(U23 = (26), 1, U23 + 1),  U23)</f>
+        <v>12</v>
+      </c>
+      <c r="V23" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A24" s="62" t="s">
+        <v>1</v>
+      </c>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="F24" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="G24" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="H24" s="47"/>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A25" s="61" t="s">
+        <v>7</v>
+      </c>
+      <c r="U25" t="str" cm="1">
+        <f t="array" aca="1" ref="U25" ca="1">INDIRECT(ADDRESS(U23, 1))</f>
+        <v>,</v>
+      </c>
+      <c r="V25" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A26" s="63" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E28" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H28" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="I28" s="48" t="s">
+        <v>60</v>
+      </c>
+      <c r="J28" s="49"/>
+      <c r="K28" s="49"/>
+      <c r="L28" s="49"/>
+      <c r="M28" s="49"/>
+      <c r="N28" s="50"/>
+      <c r="O28" s="39" t="s">
+        <v>70</v>
+      </c>
+      <c r="P28" s="40"/>
+      <c r="Q28" s="40"/>
+      <c r="R28" s="41"/>
+      <c r="S28" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E29" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="H29" s="17"/>
+      <c r="I29" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="J29" s="43"/>
+      <c r="K29" s="43"/>
+      <c r="L29" s="43"/>
+      <c r="M29" s="43"/>
+      <c r="N29" s="44"/>
+      <c r="O29" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="P29" s="31"/>
+      <c r="Q29" s="31"/>
+      <c r="R29" s="32"/>
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E30" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="H30" s="17"/>
+      <c r="I30" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="J30" s="43"/>
+      <c r="K30" s="43"/>
+      <c r="L30" s="43"/>
+      <c r="M30" s="43"/>
+      <c r="N30" s="44"/>
+      <c r="O30" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="P30" s="31"/>
+      <c r="Q30" s="31"/>
+      <c r="R30" s="32"/>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E31" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="H31" s="17"/>
+      <c r="I31" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="J31" s="43"/>
+      <c r="K31" s="43"/>
+      <c r="L31" s="43"/>
+      <c r="M31" s="43"/>
+      <c r="N31" s="44"/>
+      <c r="O31" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="P31" s="31"/>
+      <c r="Q31" s="31"/>
+      <c r="R31" s="32"/>
+    </row>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E32" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="H32" s="17"/>
+      <c r="I32" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="J32" s="43"/>
+      <c r="K32" s="43"/>
+      <c r="L32" s="43"/>
+      <c r="M32" s="43"/>
+      <c r="N32" s="44"/>
+      <c r="O32" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="P32" s="31"/>
+      <c r="Q32" s="31"/>
+      <c r="R32" s="32"/>
+    </row>
+    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E33" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="H33" s="17"/>
+      <c r="I33" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="J33" s="43"/>
+      <c r="K33" s="43"/>
+      <c r="L33" s="43"/>
+      <c r="M33" s="43"/>
+      <c r="N33" s="44"/>
+      <c r="O33" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="P33" s="31"/>
+      <c r="Q33" s="31"/>
+      <c r="R33" s="32"/>
+    </row>
+    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E34" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="H34" s="17"/>
+      <c r="I34" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="J34" s="43"/>
+      <c r="K34" s="43"/>
+      <c r="L34" s="43"/>
+      <c r="M34" s="43"/>
+      <c r="N34" s="44"/>
+      <c r="O34" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="P34" s="31"/>
+      <c r="Q34" s="31"/>
+      <c r="R34" s="32"/>
+    </row>
+    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E35" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="H35" s="17"/>
+      <c r="I35" s="42" t="s">
+        <v>65</v>
+      </c>
+      <c r="J35" s="43"/>
+      <c r="K35" s="43"/>
+      <c r="L35" s="43"/>
+      <c r="M35" s="43"/>
+      <c r="N35" s="44"/>
+      <c r="O35" s="30" t="s">
+        <v>68</v>
+      </c>
+      <c r="P35" s="31"/>
+      <c r="Q35" s="31"/>
+      <c r="R35" s="32"/>
+    </row>
+    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E36" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="H36" s="17"/>
+      <c r="I36" s="42" t="s">
+        <v>62</v>
+      </c>
+      <c r="J36" s="43"/>
+      <c r="K36" s="43"/>
+      <c r="L36" s="43"/>
+      <c r="M36" s="43"/>
+      <c r="N36" s="44"/>
+      <c r="O36" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="P36" s="31"/>
+      <c r="Q36" s="31"/>
+      <c r="R36" s="32"/>
+    </row>
+    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E37" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H37" s="17"/>
+      <c r="I37" s="42" t="s">
+        <v>61</v>
+      </c>
+      <c r="J37" s="43"/>
+      <c r="K37" s="43"/>
+      <c r="L37" s="43"/>
+      <c r="M37" s="43"/>
+      <c r="N37" s="44"/>
+      <c r="O37" s="30" t="s">
+        <v>69</v>
+      </c>
+      <c r="P37" s="31"/>
+      <c r="Q37" s="31"/>
+      <c r="R37" s="32"/>
+      <c r="W37" s="4"/>
+    </row>
+    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E38" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="H38" s="17"/>
+      <c r="I38" s="45" t="s">
+        <v>59</v>
+      </c>
+      <c r="J38" s="46"/>
+      <c r="K38" s="46"/>
+      <c r="L38" s="46"/>
+      <c r="M38" s="46"/>
+      <c r="N38" s="47"/>
+      <c r="O38" s="33" t="s">
+        <v>71</v>
+      </c>
+      <c r="P38" s="34"/>
+      <c r="Q38" s="34"/>
+      <c r="R38" s="35"/>
+    </row>
+    <row r="39" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A39" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="B39" s="37"/>
+      <c r="C39" s="37"/>
+      <c r="D39" s="38"/>
+      <c r="E39" s="36" t="s">
+        <v>46</v>
+      </c>
+      <c r="F39" s="37"/>
+      <c r="G39" s="37"/>
+      <c r="H39" s="38"/>
+      <c r="I39" s="36" t="s">
+        <v>58</v>
+      </c>
+      <c r="J39" s="37"/>
+      <c r="K39" s="37"/>
+      <c r="L39" s="37"/>
+      <c r="M39" s="37"/>
+      <c r="N39" s="38"/>
+      <c r="O39" s="36" t="s">
+        <v>72</v>
+      </c>
+      <c r="P39" s="37"/>
+      <c r="Q39" s="37"/>
+      <c r="R39" s="38"/>
+    </row>
+    <row r="43" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="45" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="46" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="40">
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="L15:M15"/>
+    <mergeCell ref="H18:M18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="G8:K9"/>
+    <mergeCell ref="K13:L13"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="E39:H39"/>
+    <mergeCell ref="A39:D39"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="I38:N38"/>
+    <mergeCell ref="I39:N39"/>
+    <mergeCell ref="I28:N28"/>
+    <mergeCell ref="I29:N29"/>
+    <mergeCell ref="I30:N30"/>
+    <mergeCell ref="I31:N31"/>
+    <mergeCell ref="I32:N32"/>
+    <mergeCell ref="I33:N33"/>
+    <mergeCell ref="O38:R38"/>
+    <mergeCell ref="O39:R39"/>
+    <mergeCell ref="O28:R28"/>
+    <mergeCell ref="O29:R29"/>
+    <mergeCell ref="O30:R30"/>
+    <mergeCell ref="O31:R31"/>
+    <mergeCell ref="O32:R32"/>
+    <mergeCell ref="O33:R33"/>
+    <mergeCell ref="O34:R34"/>
+    <mergeCell ref="O35:R35"/>
+    <mergeCell ref="O36:R36"/>
+    <mergeCell ref="O37:R37"/>
+    <mergeCell ref="I34:N34"/>
+    <mergeCell ref="I35:N35"/>
+    <mergeCell ref="I36:N36"/>
+    <mergeCell ref="I37:N37"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="G13:H13"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38C2C576-A075-4DB3-9850-67A4FFD34986}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Working on parser for eBF
</commit_message>
<xml_diff>
--- a/eBF Compiler and Parser.xlsx
+++ b/eBF Compiler and Parser.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sebastian\ePU\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SENGa\ePU\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C327AFFC-25E1-4B6B-87E6-07861F317D22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67CC31A4-C1B6-41DA-A517-3F3C202D2428}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{B06A63A8-6D73-4E43-885F-3569BFC944DC}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{B06A63A8-6D73-4E43-885F-3569BFC944DC}"/>
   </bookViews>
   <sheets>
     <sheet name="Working Sheet and Dev Notes" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="80">
   <si>
     <t>PROGRAM START</t>
   </si>
@@ -561,92 +561,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
@@ -654,6 +569,93 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -988,24 +990,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EE5DD05-ADC3-4927-894B-E00B418CFE20}">
-  <dimension ref="A1:Y46"/>
+  <dimension ref="A1:AL52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+    <sheetView tabSelected="1" topLeftCell="T13" workbookViewId="0">
+      <selection activeCell="AC19" sqref="AC19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A1" s="60" t="s">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A1" s="31" t="s">
         <v>1</v>
       </c>
       <c r="E1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A2" s="61" t="s">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A2" s="32" t="s">
         <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
@@ -1018,8 +1020,8 @@
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A3" s="61" t="s">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A3" s="32" t="s">
         <v>1</v>
       </c>
       <c r="E3" s="3" t="s">
@@ -1032,8 +1034,8 @@
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A4" s="61" t="s">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A4" s="32" t="s">
         <v>1</v>
       </c>
       <c r="E4" s="3" t="s">
@@ -1046,8 +1048,8 @@
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A5" s="61" t="s">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A5" s="32" t="s">
         <v>1</v>
       </c>
       <c r="E5" s="3" t="s">
@@ -1063,8 +1065,8 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="61" t="s">
+    <row r="6" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="32" t="s">
         <v>3</v>
       </c>
       <c r="E6" s="3" t="s">
@@ -1090,8 +1092,8 @@
       <c r="X6" s="8"/>
       <c r="Y6" s="16"/>
     </row>
-    <row r="7" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="61" t="s">
+    <row r="7" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="32" t="s">
         <v>3</v>
       </c>
       <c r="E7" s="3" t="s">
@@ -1118,15 +1120,15 @@
       </c>
       <c r="W7" cm="1">
         <f t="array" aca="1" ref="W7" ca="1">INDIRECT(ADDRESS(V10, V9 + S11))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X7" t="s">
         <v>32</v>
       </c>
       <c r="Y7" s="17"/>
     </row>
-    <row r="8" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="61" t="s">
+    <row r="8" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="32" t="s">
         <v>1</v>
       </c>
       <c r="E8" s="3" t="s">
@@ -1135,18 +1137,18 @@
       <c r="F8" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="G8" s="29" t="s">
+      <c r="G8" s="54" t="s">
         <v>74</v>
       </c>
-      <c r="H8" s="57"/>
-      <c r="I8" s="57"/>
-      <c r="J8" s="57"/>
-      <c r="K8" s="57"/>
+      <c r="H8" s="55"/>
+      <c r="I8" s="55"/>
+      <c r="J8" s="55"/>
+      <c r="K8" s="55"/>
       <c r="O8" s="3"/>
       <c r="Y8" s="17"/>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A9" s="61" t="s">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A9" s="32" t="s">
         <v>7</v>
       </c>
       <c r="E9" s="5" t="s">
@@ -1155,11 +1157,11 @@
       <c r="F9" s="15">
         <v>1000</v>
       </c>
-      <c r="G9" s="29"/>
-      <c r="H9" s="57"/>
-      <c r="I9" s="57"/>
-      <c r="J9" s="57"/>
-      <c r="K9" s="57"/>
+      <c r="G9" s="54"/>
+      <c r="H9" s="55"/>
+      <c r="I9" s="55"/>
+      <c r="J9" s="55"/>
+      <c r="K9" s="55"/>
       <c r="O9" s="3"/>
       <c r="Q9">
         <v>1010</v>
@@ -1175,8 +1177,8 @@
       </c>
       <c r="Y9" s="17"/>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A10" s="61" t="s">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A10" s="32" t="s">
         <v>4</v>
       </c>
       <c r="E10" t="s">
@@ -1191,8 +1193,8 @@
       </c>
       <c r="Y10" s="17"/>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A11" s="61" t="s">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A11" s="32" t="s">
         <v>2</v>
       </c>
       <c r="E11" s="1" t="s">
@@ -1209,19 +1211,19 @@
       </c>
       <c r="Q11" t="str">
         <f ca="1">MID(Q9, S11, 1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S11">
         <f ca="1">IF(J20 = 1, IF(S11 = (LEN(Q9) + 1), 1, S11 + 1),  S11)</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="T11" t="s">
         <v>37</v>
       </c>
       <c r="Y11" s="17"/>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A12" s="61" t="s">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A12" s="32" t="s">
         <v>7</v>
       </c>
       <c r="E12" s="3" t="s">
@@ -1232,12 +1234,12 @@
       </c>
       <c r="G12" s="20"/>
       <c r="H12" s="7"/>
-      <c r="I12" s="55"/>
+      <c r="I12" s="4"/>
       <c r="O12" s="3"/>
       <c r="Y12" s="17"/>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A13" s="61" t="s">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A13" s="32" t="s">
         <v>3</v>
       </c>
       <c r="E13" s="3" t="s">
@@ -1246,18 +1248,18 @@
       <c r="F13" s="14">
         <v>1011</v>
       </c>
-      <c r="G13" s="49" t="s">
+      <c r="G13" s="41" t="s">
         <v>77</v>
       </c>
-      <c r="H13" s="49"/>
+      <c r="H13" s="41"/>
       <c r="I13" s="56" t="s">
         <v>78</v>
       </c>
       <c r="J13" s="56"/>
-      <c r="K13" s="37" t="s">
+      <c r="K13" s="46" t="s">
         <v>76</v>
       </c>
-      <c r="L13" s="38"/>
+      <c r="L13" s="47"/>
       <c r="O13" s="3"/>
       <c r="Q13">
         <v>1</v>
@@ -1274,8 +1276,8 @@
       </c>
       <c r="Y13" s="17"/>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A14" s="61" t="s">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A14" s="32" t="s">
         <v>3</v>
       </c>
       <c r="E14" s="3" t="s">
@@ -1284,10 +1286,10 @@
       <c r="F14" s="14">
         <v>1100</v>
       </c>
-      <c r="G14" s="53" t="s">
+      <c r="G14" s="39" t="s">
         <v>76</v>
       </c>
-      <c r="H14" s="52"/>
+      <c r="H14" s="40"/>
       <c r="I14" s="21"/>
       <c r="O14" s="3"/>
       <c r="V14">
@@ -1299,8 +1301,8 @@
       </c>
       <c r="Y14" s="17"/>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A15" s="61" t="s">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A15" s="32" t="s">
         <v>7</v>
       </c>
       <c r="E15" s="3" t="s">
@@ -1309,13 +1311,13 @@
       <c r="F15" s="14">
         <v>1101</v>
       </c>
-      <c r="G15" s="51" t="s">
+      <c r="G15" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="H15" s="54" t="s">
+      <c r="H15" s="62" t="s">
         <v>22</v>
       </c>
-      <c r="I15" s="54"/>
+      <c r="I15" s="62"/>
       <c r="J15" s="56" t="s">
         <v>22</v>
       </c>
@@ -1323,20 +1325,20 @@
       <c r="L15" s="56" t="s">
         <v>22</v>
       </c>
-      <c r="M15" s="58"/>
+      <c r="M15" s="63"/>
       <c r="O15" s="3"/>
       <c r="Q15">
         <f ca="1">IF(J20 = 1, IF(Q15 &gt;= Q13, 0, Q15 + 1), Q15)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S15" t="str">
         <f ca="1">IF(Q15 = Q13, IF(LEN(S15) = LEN(Q9), "", S15 &amp; Q11), S15)</f>
-        <v>1010</v>
+        <v>1</v>
       </c>
       <c r="Y15" s="17"/>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A16" s="61" t="s">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A16" s="32" t="s">
         <v>4</v>
       </c>
       <c r="E16" s="3" t="s">
@@ -1362,8 +1364,8 @@
       <c r="X16" s="6"/>
       <c r="Y16" s="19"/>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A17" s="61" t="s">
+    <row r="17" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="A17" s="32" t="s">
         <v>2</v>
       </c>
       <c r="E17" s="9" t="s">
@@ -1374,25 +1376,25 @@
       </c>
       <c r="G17" s="19"/>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A18" s="61" t="s">
+    <row r="18" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="A18" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="E18" s="36" t="s">
+      <c r="E18" s="45" t="s">
         <v>29</v>
       </c>
-      <c r="F18" s="37"/>
-      <c r="G18" s="59">
+      <c r="F18" s="46"/>
+      <c r="G18" s="30">
         <v>1111</v>
       </c>
-      <c r="H18" s="37" t="s">
+      <c r="H18" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="I18" s="37"/>
-      <c r="J18" s="37"/>
-      <c r="K18" s="37"/>
-      <c r="L18" s="37"/>
-      <c r="M18" s="38"/>
+      <c r="I18" s="46"/>
+      <c r="J18" s="46"/>
+      <c r="K18" s="46"/>
+      <c r="L18" s="46"/>
+      <c r="M18" s="47"/>
       <c r="N18" s="4"/>
       <c r="O18" s="4"/>
       <c r="Q18" s="4"/>
@@ -1400,18 +1402,18 @@
       <c r="S18" s="4"/>
       <c r="T18" s="4"/>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A19" s="61" t="s">
+    <row r="19" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="A19" s="32" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A20" s="61" t="s">
+    <row r="20" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="A20" s="32" t="s">
         <v>3</v>
       </c>
       <c r="J20">
         <f ca="1">IF(J20=0, 1, 0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K20" t="s">
         <v>27</v>
@@ -1420,22 +1422,22 @@
       <c r="P20" s="4"/>
       <c r="R20" s="4"/>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A21" s="61" t="s">
+    <row r="21" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="A21" s="32" t="s">
         <v>1</v>
       </c>
       <c r="E21" s="24" t="s">
         <v>57</v>
       </c>
       <c r="F21" s="28"/>
-      <c r="G21" s="37" t="s">
+      <c r="G21" s="46" t="s">
         <v>56</v>
       </c>
-      <c r="H21" s="38"/>
+      <c r="H21" s="47"/>
       <c r="R21" s="4"/>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A22" s="61" t="s">
+    <row r="22" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="A22" s="32" t="s">
         <v>1</v>
       </c>
       <c r="D22" s="4"/>
@@ -1445,16 +1447,16 @@
       <c r="F22" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="G22" s="48" t="s">
+      <c r="G22" s="59" t="s">
         <v>50</v>
       </c>
-      <c r="H22" s="50"/>
+      <c r="H22" s="60"/>
       <c r="I22" s="4"/>
       <c r="N22" s="4"/>
       <c r="Q22" s="4"/>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A23" s="61" t="s">
+    <row r="23" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="A23" s="32" t="s">
         <v>1</v>
       </c>
       <c r="E23" s="25" t="s">
@@ -1463,20 +1465,20 @@
       <c r="F23" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="G23" s="42" t="s">
+      <c r="G23" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="H23" s="44"/>
+      <c r="H23" s="38"/>
       <c r="U23">
         <f ca="1">IF(J20 = 1, IF(U23 = (26), 1, U23 + 1),  U23)</f>
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="V23" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A24" s="62" t="s">
+    <row r="24" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="A24" s="33" t="s">
         <v>1</v>
       </c>
       <c r="B24" s="4"/>
@@ -1488,29 +1490,143 @@
       <c r="F24" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="G24" s="45" t="s">
+      <c r="G24" s="57" t="s">
         <v>51</v>
       </c>
-      <c r="H24" s="47"/>
-    </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A25" s="61" t="s">
+      <c r="H24" s="58"/>
+    </row>
+    <row r="25" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="A25" s="32" t="s">
         <v>7</v>
       </c>
       <c r="U25" t="str" cm="1">
         <f t="array" aca="1" ref="U25" ca="1">INDIRECT(ADDRESS(U23, 1))</f>
-        <v>,</v>
+        <v>&lt;</v>
       </c>
       <c r="V25" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A26" s="63" t="s">
+      <c r="Y25" s="35" cm="1">
+        <f t="array" aca="1" ref="Y25:AL25" ca="1">IF(U25 = Y27:AL27, 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="Z25" s="35">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="AA25" s="35">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="AB25" s="35">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
+      <c r="AC25" s="35">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="AD25" s="35">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="AE25" s="35">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="AF25" s="35">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="AG25" s="35">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="AH25" s="35">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="AI25" s="35">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="AJ25" s="35">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="AK25" s="35">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="AL25" s="35">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="A26" s="34" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="Y26" s="35"/>
+      <c r="Z26" s="35"/>
+      <c r="AA26" s="35"/>
+      <c r="AB26" s="35"/>
+      <c r="AC26" s="35"/>
+      <c r="AD26" s="35"/>
+      <c r="AE26" s="35"/>
+      <c r="AF26" s="35"/>
+      <c r="AG26" s="35"/>
+      <c r="AH26" s="35"/>
+      <c r="AI26" s="35"/>
+      <c r="AJ26" s="35"/>
+      <c r="AK26" s="35"/>
+      <c r="AL26" s="35"/>
+    </row>
+    <row r="27" spans="1:38" x14ac:dyDescent="0.3">
+      <c r="Y27" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z27" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA27" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB27" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="AC27" s="35" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD27" s="35" t="s">
+        <v>6</v>
+      </c>
+      <c r="AE27" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="AF27" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="AG27" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="AH27" s="35" t="s">
+        <v>10</v>
+      </c>
+      <c r="AI27" s="35" t="s">
+        <v>11</v>
+      </c>
+      <c r="AJ27" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="AK27" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="AL27" s="35" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="28" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>11</v>
       </c>
@@ -1535,25 +1651,25 @@
       <c r="H28" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="I28" s="48" t="s">
+      <c r="I28" s="59" t="s">
         <v>60</v>
       </c>
-      <c r="J28" s="49"/>
-      <c r="K28" s="49"/>
-      <c r="L28" s="49"/>
-      <c r="M28" s="49"/>
-      <c r="N28" s="50"/>
-      <c r="O28" s="39" t="s">
+      <c r="J28" s="41"/>
+      <c r="K28" s="41"/>
+      <c r="L28" s="41"/>
+      <c r="M28" s="41"/>
+      <c r="N28" s="60"/>
+      <c r="O28" s="48" t="s">
         <v>70</v>
       </c>
-      <c r="P28" s="40"/>
-      <c r="Q28" s="40"/>
-      <c r="R28" s="41"/>
+      <c r="P28" s="49"/>
+      <c r="Q28" s="49"/>
+      <c r="R28" s="50"/>
       <c r="S28" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
         <v>1</v>
       </c>
@@ -1561,22 +1677,22 @@
         <v>15</v>
       </c>
       <c r="H29" s="17"/>
-      <c r="I29" s="42" t="s">
+      <c r="I29" s="36" t="s">
         <v>63</v>
       </c>
-      <c r="J29" s="43"/>
-      <c r="K29" s="43"/>
-      <c r="L29" s="43"/>
-      <c r="M29" s="43"/>
-      <c r="N29" s="44"/>
-      <c r="O29" s="30" t="s">
+      <c r="J29" s="37"/>
+      <c r="K29" s="37"/>
+      <c r="L29" s="37"/>
+      <c r="M29" s="37"/>
+      <c r="N29" s="38"/>
+      <c r="O29" s="51" t="s">
         <v>66</v>
       </c>
-      <c r="P29" s="31"/>
-      <c r="Q29" s="31"/>
-      <c r="R29" s="32"/>
-    </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="P29" s="52"/>
+      <c r="Q29" s="52"/>
+      <c r="R29" s="53"/>
+    </row>
+    <row r="30" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>1</v>
       </c>
@@ -1584,22 +1700,22 @@
         <v>15</v>
       </c>
       <c r="H30" s="17"/>
-      <c r="I30" s="42" t="s">
+      <c r="I30" s="36" t="s">
         <v>63</v>
       </c>
-      <c r="J30" s="43"/>
-      <c r="K30" s="43"/>
-      <c r="L30" s="43"/>
-      <c r="M30" s="43"/>
-      <c r="N30" s="44"/>
-      <c r="O30" s="30" t="s">
+      <c r="J30" s="37"/>
+      <c r="K30" s="37"/>
+      <c r="L30" s="37"/>
+      <c r="M30" s="37"/>
+      <c r="N30" s="38"/>
+      <c r="O30" s="51" t="s">
         <v>66</v>
       </c>
-      <c r="P30" s="31"/>
-      <c r="Q30" s="31"/>
-      <c r="R30" s="32"/>
-    </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="P30" s="52"/>
+      <c r="Q30" s="52"/>
+      <c r="R30" s="53"/>
+    </row>
+    <row r="31" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>1</v>
       </c>
@@ -1607,22 +1723,22 @@
         <v>15</v>
       </c>
       <c r="H31" s="17"/>
-      <c r="I31" s="42" t="s">
+      <c r="I31" s="36" t="s">
         <v>63</v>
       </c>
-      <c r="J31" s="43"/>
-      <c r="K31" s="43"/>
-      <c r="L31" s="43"/>
-      <c r="M31" s="43"/>
-      <c r="N31" s="44"/>
-      <c r="O31" s="30" t="s">
+      <c r="J31" s="37"/>
+      <c r="K31" s="37"/>
+      <c r="L31" s="37"/>
+      <c r="M31" s="37"/>
+      <c r="N31" s="38"/>
+      <c r="O31" s="51" t="s">
         <v>66</v>
       </c>
-      <c r="P31" s="31"/>
-      <c r="Q31" s="31"/>
-      <c r="R31" s="32"/>
-    </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="P31" s="52"/>
+      <c r="Q31" s="52"/>
+      <c r="R31" s="53"/>
+    </row>
+    <row r="32" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
         <v>3</v>
       </c>
@@ -1630,22 +1746,22 @@
         <v>17</v>
       </c>
       <c r="H32" s="17"/>
-      <c r="I32" s="42" t="s">
+      <c r="I32" s="36" t="s">
         <v>64</v>
       </c>
-      <c r="J32" s="43"/>
-      <c r="K32" s="43"/>
-      <c r="L32" s="43"/>
-      <c r="M32" s="43"/>
-      <c r="N32" s="44"/>
-      <c r="O32" s="30" t="s">
+      <c r="J32" s="37"/>
+      <c r="K32" s="37"/>
+      <c r="L32" s="37"/>
+      <c r="M32" s="37"/>
+      <c r="N32" s="38"/>
+      <c r="O32" s="51" t="s">
         <v>67</v>
       </c>
-      <c r="P32" s="31"/>
-      <c r="Q32" s="31"/>
-      <c r="R32" s="32"/>
-    </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="P32" s="52"/>
+      <c r="Q32" s="52"/>
+      <c r="R32" s="53"/>
+    </row>
+    <row r="33" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
         <v>3</v>
       </c>
@@ -1653,22 +1769,22 @@
         <v>17</v>
       </c>
       <c r="H33" s="17"/>
-      <c r="I33" s="42" t="s">
+      <c r="I33" s="36" t="s">
         <v>64</v>
       </c>
-      <c r="J33" s="43"/>
-      <c r="K33" s="43"/>
-      <c r="L33" s="43"/>
-      <c r="M33" s="43"/>
-      <c r="N33" s="44"/>
-      <c r="O33" s="30" t="s">
+      <c r="J33" s="37"/>
+      <c r="K33" s="37"/>
+      <c r="L33" s="37"/>
+      <c r="M33" s="37"/>
+      <c r="N33" s="38"/>
+      <c r="O33" s="51" t="s">
         <v>67</v>
       </c>
-      <c r="P33" s="31"/>
-      <c r="Q33" s="31"/>
-      <c r="R33" s="32"/>
-    </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="P33" s="52"/>
+      <c r="Q33" s="52"/>
+      <c r="R33" s="53"/>
+    </row>
+    <row r="34" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
         <v>1</v>
       </c>
@@ -1676,22 +1792,22 @@
         <v>15</v>
       </c>
       <c r="H34" s="17"/>
-      <c r="I34" s="42" t="s">
+      <c r="I34" s="36" t="s">
         <v>63</v>
       </c>
-      <c r="J34" s="43"/>
-      <c r="K34" s="43"/>
-      <c r="L34" s="43"/>
-      <c r="M34" s="43"/>
-      <c r="N34" s="44"/>
-      <c r="O34" s="30" t="s">
+      <c r="J34" s="37"/>
+      <c r="K34" s="37"/>
+      <c r="L34" s="37"/>
+      <c r="M34" s="37"/>
+      <c r="N34" s="38"/>
+      <c r="O34" s="51" t="s">
         <v>66</v>
       </c>
-      <c r="P34" s="31"/>
-      <c r="Q34" s="31"/>
-      <c r="R34" s="32"/>
-    </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="P34" s="52"/>
+      <c r="Q34" s="52"/>
+      <c r="R34" s="53"/>
+    </row>
+    <row r="35" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
         <v>4</v>
       </c>
@@ -1699,22 +1815,22 @@
         <v>18</v>
       </c>
       <c r="H35" s="17"/>
-      <c r="I35" s="42" t="s">
+      <c r="I35" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="J35" s="43"/>
-      <c r="K35" s="43"/>
-      <c r="L35" s="43"/>
-      <c r="M35" s="43"/>
-      <c r="N35" s="44"/>
-      <c r="O35" s="30" t="s">
+      <c r="J35" s="37"/>
+      <c r="K35" s="37"/>
+      <c r="L35" s="37"/>
+      <c r="M35" s="37"/>
+      <c r="N35" s="38"/>
+      <c r="O35" s="51" t="s">
         <v>68</v>
       </c>
-      <c r="P35" s="31"/>
-      <c r="Q35" s="31"/>
-      <c r="R35" s="32"/>
-    </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="P35" s="52"/>
+      <c r="Q35" s="52"/>
+      <c r="R35" s="53"/>
+    </row>
+    <row r="36" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
         <v>7</v>
       </c>
@@ -1722,22 +1838,22 @@
         <v>21</v>
       </c>
       <c r="H36" s="17"/>
-      <c r="I36" s="42" t="s">
+      <c r="I36" s="36" t="s">
         <v>62</v>
       </c>
-      <c r="J36" s="43"/>
-      <c r="K36" s="43"/>
-      <c r="L36" s="43"/>
-      <c r="M36" s="43"/>
-      <c r="N36" s="44"/>
-      <c r="O36" s="30" t="s">
+      <c r="J36" s="37"/>
+      <c r="K36" s="37"/>
+      <c r="L36" s="37"/>
+      <c r="M36" s="37"/>
+      <c r="N36" s="38"/>
+      <c r="O36" s="51" t="s">
         <v>73</v>
       </c>
-      <c r="P36" s="31"/>
-      <c r="Q36" s="31"/>
-      <c r="R36" s="32"/>
-    </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="P36" s="52"/>
+      <c r="Q36" s="52"/>
+      <c r="R36" s="53"/>
+    </row>
+    <row r="37" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
         <v>12</v>
       </c>
@@ -1751,23 +1867,23 @@
         <v>15</v>
       </c>
       <c r="H37" s="17"/>
-      <c r="I37" s="42" t="s">
+      <c r="I37" s="36" t="s">
         <v>61</v>
       </c>
-      <c r="J37" s="43"/>
-      <c r="K37" s="43"/>
-      <c r="L37" s="43"/>
-      <c r="M37" s="43"/>
-      <c r="N37" s="44"/>
-      <c r="O37" s="30" t="s">
+      <c r="J37" s="37"/>
+      <c r="K37" s="37"/>
+      <c r="L37" s="37"/>
+      <c r="M37" s="37"/>
+      <c r="N37" s="38"/>
+      <c r="O37" s="51" t="s">
         <v>69</v>
       </c>
-      <c r="P37" s="31"/>
-      <c r="Q37" s="31"/>
-      <c r="R37" s="32"/>
+      <c r="P37" s="52"/>
+      <c r="Q37" s="52"/>
+      <c r="R37" s="53"/>
       <c r="W37" s="4"/>
     </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
         <v>14</v>
       </c>
@@ -1775,75 +1891,76 @@
         <v>45</v>
       </c>
       <c r="H38" s="17"/>
-      <c r="I38" s="45" t="s">
+      <c r="I38" s="57" t="s">
         <v>59</v>
       </c>
-      <c r="J38" s="46"/>
-      <c r="K38" s="46"/>
-      <c r="L38" s="46"/>
-      <c r="M38" s="46"/>
-      <c r="N38" s="47"/>
-      <c r="O38" s="33" t="s">
+      <c r="J38" s="61"/>
+      <c r="K38" s="61"/>
+      <c r="L38" s="61"/>
+      <c r="M38" s="61"/>
+      <c r="N38" s="58"/>
+      <c r="O38" s="42" t="s">
         <v>71</v>
       </c>
-      <c r="P38" s="34"/>
-      <c r="Q38" s="34"/>
-      <c r="R38" s="35"/>
-    </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A39" s="36" t="s">
+      <c r="P38" s="43"/>
+      <c r="Q38" s="43"/>
+      <c r="R38" s="44"/>
+    </row>
+    <row r="39" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A39" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="B39" s="37"/>
-      <c r="C39" s="37"/>
-      <c r="D39" s="38"/>
-      <c r="E39" s="36" t="s">
+      <c r="B39" s="46"/>
+      <c r="C39" s="46"/>
+      <c r="D39" s="47"/>
+      <c r="E39" s="45" t="s">
         <v>46</v>
       </c>
-      <c r="F39" s="37"/>
-      <c r="G39" s="37"/>
-      <c r="H39" s="38"/>
-      <c r="I39" s="36" t="s">
+      <c r="F39" s="46"/>
+      <c r="G39" s="46"/>
+      <c r="H39" s="47"/>
+      <c r="I39" s="45" t="s">
         <v>58</v>
       </c>
-      <c r="J39" s="37"/>
-      <c r="K39" s="37"/>
-      <c r="L39" s="37"/>
-      <c r="M39" s="37"/>
-      <c r="N39" s="38"/>
-      <c r="O39" s="36" t="s">
+      <c r="J39" s="46"/>
+      <c r="K39" s="46"/>
+      <c r="L39" s="46"/>
+      <c r="M39" s="46"/>
+      <c r="N39" s="47"/>
+      <c r="O39" s="45" t="s">
         <v>72</v>
       </c>
-      <c r="P39" s="37"/>
-      <c r="Q39" s="37"/>
-      <c r="R39" s="38"/>
-    </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="P39" s="46"/>
+      <c r="Q39" s="46"/>
+      <c r="R39" s="47"/>
+    </row>
+    <row r="43" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>55</v>
       </c>
     </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="L15:M15"/>
-    <mergeCell ref="H18:M18"/>
     <mergeCell ref="E18:F18"/>
     <mergeCell ref="G8:K9"/>
     <mergeCell ref="K13:L13"/>
@@ -1861,8 +1978,6 @@
     <mergeCell ref="I30:N30"/>
     <mergeCell ref="I31:N31"/>
     <mergeCell ref="I32:N32"/>
-    <mergeCell ref="I33:N33"/>
-    <mergeCell ref="O38:R38"/>
     <mergeCell ref="O39:R39"/>
     <mergeCell ref="O28:R28"/>
     <mergeCell ref="O29:R29"/>
@@ -1874,12 +1989,18 @@
     <mergeCell ref="O35:R35"/>
     <mergeCell ref="O36:R36"/>
     <mergeCell ref="O37:R37"/>
+    <mergeCell ref="I37:N37"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="I33:N33"/>
+    <mergeCell ref="O38:R38"/>
     <mergeCell ref="I34:N34"/>
     <mergeCell ref="I35:N35"/>
     <mergeCell ref="I36:N36"/>
-    <mergeCell ref="I37:N37"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="L15:M15"/>
+    <mergeCell ref="H18:M18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1891,7 +2012,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>